<commit_message>
Added technology concepts for low emission small-scale fluidised bed combustion systems. Added further biomass product caegories for these systems.
</commit_message>
<xml_diff>
--- a/src/Biomass_Data.xlsx
+++ b/src/Biomass_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="6480" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="6480" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Potentials" sheetId="1" r:id="rId1"/>
@@ -234,7 +234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="152">
   <si>
     <t>Stroh</t>
   </si>
@@ -703,14 +703,33 @@
   <si>
     <t>MAX (Energetische Nutzung 2015 Max + Mobilisierbares Potential Max)</t>
   </si>
+  <si>
+    <t>Hay pellet</t>
+  </si>
+  <si>
+    <t>Kohle</t>
+  </si>
+  <si>
+    <t>Müll</t>
+  </si>
+  <si>
+    <t>Özge Mutlu (SmartWirbelschicht)</t>
+  </si>
+  <si>
+    <t>Foliage pellets</t>
+  </si>
+  <si>
+    <t>Laub</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1045,7 +1064,7 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1317,6 +1336,10 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1330,6 +1353,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1754,13 +1783,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
       <c r="G2" s="39"/>
     </row>
     <row r="3" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1950,13 +1979,13 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="123" t="s">
+      <c r="B12" s="125" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="124"/>
-      <c r="D12" s="124"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="124"/>
+      <c r="C12" s="126"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:8" ht="21" x14ac:dyDescent="0.25">
@@ -2138,13 +2167,13 @@
       </c>
     </row>
     <row r="22" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="124" t="s">
+      <c r="B22" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="124"/>
-      <c r="D22" s="124"/>
-      <c r="E22" s="124"/>
-      <c r="F22" s="124"/>
+      <c r="C22" s="126"/>
+      <c r="D22" s="126"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="126"/>
       <c r="G22" s="11"/>
       <c r="H22" s="1"/>
     </row>
@@ -2228,7 +2257,7 @@
         <v>101</v>
       </c>
       <c r="C27" s="95">
-        <f>CulStart!Z7/Potentials!C10</f>
+        <f>CulStart!AD7/Potentials!C10</f>
         <v>0.5629704166666667</v>
       </c>
       <c r="D27" s="95"/>
@@ -2246,7 +2275,7 @@
         <v>102</v>
       </c>
       <c r="C28" s="95">
-        <f>CulStart!Z7/Potentials!C11</f>
+        <f>CulStart!AD7/Potentials!C11</f>
         <v>0.5629704166666667</v>
       </c>
       <c r="D28" s="95"/>
@@ -2260,13 +2289,13 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="125" t="s">
+      <c r="B29" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="125"/>
-      <c r="D29" s="125"/>
-      <c r="E29" s="125"/>
-      <c r="F29" s="125"/>
+      <c r="C29" s="127"/>
+      <c r="D29" s="127"/>
+      <c r="E29" s="127"/>
+      <c r="F29" s="127"/>
     </row>
     <row r="30" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
@@ -2346,7 +2375,7 @@
         <v>101</v>
       </c>
       <c r="C34" s="95">
-        <f>CulStart!Z7/Potentials!C20</f>
+        <f>CulStart!AD7/Potentials!C20</f>
         <v>0.5629704166666667</v>
       </c>
       <c r="D34" s="95"/>
@@ -2364,7 +2393,7 @@
         <v>102</v>
       </c>
       <c r="C35" s="95">
-        <f>CulStart!Z7/Potentials!C21</f>
+        <f>CulStart!AD7/Potentials!C21</f>
         <v>0.5629704166666667</v>
       </c>
       <c r="D35" s="95"/>
@@ -2392,10 +2421,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N32"/>
+  <dimension ref="B1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2431,20 +2460,20 @@
         <v>6</v>
       </c>
       <c r="C3" s="107">
-        <f>SUM(C5:C15)</f>
-        <v>519.02304319999996</v>
+        <f>SUM(C5:C16)</f>
+        <v>519.02804319999996</v>
       </c>
       <c r="D3" s="107">
-        <f>SUM(D5:D15)</f>
-        <v>519.02304319999996</v>
+        <f>SUM(D5:D16)</f>
+        <v>519.02804319999996</v>
       </c>
       <c r="E3" s="107">
-        <f>SUM(E5:E15)</f>
-        <v>519.02304319999996</v>
+        <f>SUM(E5:E16)</f>
+        <v>519.02804319999996</v>
       </c>
       <c r="F3" s="107">
-        <f>SUM(F5:F15)</f>
-        <v>519.02304319999996</v>
+        <f>SUM(F5:F16)</f>
+        <v>519.02804319999996</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="21" x14ac:dyDescent="0.25">
@@ -2654,344 +2683,385 @@
       </c>
     </row>
     <row r="14" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B14" s="109" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="110">
+      <c r="B14" s="101" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="130">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D14" s="130">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E14" s="130">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F14" s="130">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B15" s="109" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="110">
         <v>1</v>
       </c>
-      <c r="D14" s="110">
+      <c r="D15" s="110">
         <v>1</v>
       </c>
-      <c r="E14" s="110">
+      <c r="E15" s="110">
         <v>1</v>
       </c>
-      <c r="F14" s="110">
+      <c r="F15" s="110">
         <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="105" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="108">
-        <v>36</v>
-      </c>
-      <c r="D15" s="108">
-        <v>36</v>
-      </c>
-      <c r="E15" s="108">
-        <v>36</v>
-      </c>
-      <c r="F15" s="108">
-        <v>36</v>
       </c>
       <c r="G15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="C16" s="99"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="16" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="108">
+        <v>36</v>
+      </c>
+      <c r="D16" s="108">
+        <v>36</v>
+      </c>
+      <c r="E16" s="108">
+        <v>36</v>
+      </c>
+      <c r="F16" s="108">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="C17" s="99"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B19" s="102" t="s">
+    <row r="20" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B20" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="106">
+      <c r="C20" s="106">
         <v>2015</v>
       </c>
-      <c r="D19" s="106">
+      <c r="D20" s="106">
         <v>2020</v>
       </c>
-      <c r="E19" s="106">
+      <c r="E20" s="106">
         <v>2030</v>
       </c>
-      <c r="F19" s="106">
+      <c r="F20" s="106">
         <v>2050</v>
       </c>
     </row>
-    <row r="20" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="103" t="s">
+    <row r="21" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="107">
-        <f>SUM(C22:C32)</f>
-        <v>657.04140204399994</v>
-      </c>
-      <c r="D20" s="107">
-        <f>SUM(D22:D32)</f>
-        <v>844.95760964873148</v>
-      </c>
-      <c r="E20" s="107">
-        <f>SUM(E22:E32)</f>
-        <v>1220.7900248581946</v>
-      </c>
-      <c r="F20" s="107">
-        <f>SUM(F22:F32)</f>
-        <v>1220.7900248581946</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B21" s="104" t="s">
+      <c r="C21" s="107">
+        <f>SUM(C23:C34)</f>
+        <v>657.06510204400001</v>
+      </c>
+      <c r="D21" s="107">
+        <f>SUM(D23:D34)</f>
+        <v>845.03844298206491</v>
+      </c>
+      <c r="E21" s="107">
+        <f>SUM(E23:E34)</f>
+        <v>1220.9851248581945</v>
+      </c>
+      <c r="F21" s="107">
+        <f>SUM(F23:F34)</f>
+        <v>1220.9851248581945</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B22" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="99">
-        <f>SUM(C22:C30)</f>
+      <c r="C22" s="99">
+        <f>SUM(C23:C31)</f>
         <v>486.04140204399994</v>
       </c>
-      <c r="D21" s="99">
-        <f>SUM(D22:D30)</f>
+      <c r="D22" s="99">
+        <f>SUM(D23:D31)</f>
         <v>550.95760964873148</v>
       </c>
-      <c r="E21" s="99">
-        <f>SUM(E22:E30)</f>
+      <c r="E22" s="99">
+        <f>SUM(E23:E31)</f>
         <v>680.79002485819444</v>
       </c>
-      <c r="F21" s="99">
-        <f>SUM(F22:F30)</f>
+      <c r="F22" s="99">
+        <f>SUM(F23:F31)</f>
         <v>680.79002485819444</v>
       </c>
     </row>
-    <row r="22" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B22" s="100" t="s">
+    <row r="23" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B23" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="120">
+      <c r="C23" s="120">
         <v>150</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D23" s="25">
         <v>150</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E23" s="25">
         <v>150</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F23" s="25">
         <v>150</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B23" s="101" t="s">
-        <v>110</v>
-      </c>
-      <c r="C23" s="112">
-        <v>24.067606464000001</v>
-      </c>
-      <c r="D23" s="111">
-        <f t="shared" ref="D23:D32" si="0">C23+(E23-C23)/3</f>
-        <v>63.518032329129724</v>
-      </c>
-      <c r="E23" s="111">
-        <v>142.41888405938917</v>
-      </c>
-      <c r="F23" s="111">
-        <v>142.41888405938917</v>
-      </c>
-      <c r="G23" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="B24" s="101" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="112">
+        <v>24.067606464000001</v>
+      </c>
+      <c r="D24" s="111">
+        <f t="shared" ref="D24:D34" si="0">C24+(E24-C24)/3</f>
+        <v>63.518032329129724</v>
+      </c>
+      <c r="E24" s="111">
+        <v>142.41888405938917</v>
+      </c>
+      <c r="F24" s="111">
+        <v>142.41888405938917</v>
+      </c>
+      <c r="G24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B25" s="101" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="112">
+      <c r="C25" s="112">
         <v>33.590752380000005</v>
       </c>
-      <c r="D24" s="111">
+      <c r="D25" s="111">
         <f t="shared" si="0"/>
         <v>50.076235608920641</v>
       </c>
-      <c r="E24" s="111">
+      <c r="E25" s="111">
         <v>83.047202066761912</v>
       </c>
-      <c r="F24" s="111">
+      <c r="F25" s="111">
         <v>83.047202066761912</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B25" s="101" t="s">
+    <row r="26" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B26" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="112">
+      <c r="C26" s="112">
         <v>8.4913919999999994</v>
       </c>
-      <c r="D25" s="111">
+      <c r="D26" s="111">
         <f t="shared" si="0"/>
         <v>8.4913919999999994</v>
       </c>
-      <c r="E25" s="111">
+      <c r="E26" s="111">
         <v>8.4913919999999994</v>
       </c>
-      <c r="F25" s="111">
+      <c r="F26" s="111">
         <v>8.4913919999999994</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G26" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B26" s="113" t="s">
+    <row r="27" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B27" s="113" t="s">
         <v>117</v>
       </c>
-      <c r="C26" s="112">
+      <c r="C27" s="112">
         <v>68.515977599999999</v>
       </c>
-      <c r="D26" s="111">
+      <c r="D27" s="111">
         <f t="shared" si="0"/>
         <v>68.515977599999999</v>
       </c>
-      <c r="E26" s="111">
+      <c r="E27" s="111">
         <v>68.515977599999999</v>
       </c>
-      <c r="F26" s="111">
+      <c r="F27" s="111">
         <v>68.515977599999999</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B27" s="101" t="s">
+    <row r="28" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B28" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="112">
+      <c r="C28" s="112">
         <v>88.240319999999997</v>
       </c>
-      <c r="D27" s="111">
+      <c r="D28" s="111">
         <f t="shared" si="0"/>
         <v>88.240319999999997</v>
       </c>
-      <c r="E27" s="111">
+      <c r="E28" s="111">
         <v>88.240319999999997</v>
       </c>
-      <c r="F27" s="111">
+      <c r="F28" s="111">
         <v>88.240319999999997</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B28" s="101" t="s">
+    <row r="29" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B29" s="101" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="112">
+      <c r="C29" s="112">
         <v>40.132713600000002</v>
       </c>
-      <c r="D28" s="111">
+      <c r="D29" s="111">
         <f t="shared" si="0"/>
         <v>45.106345444014494</v>
       </c>
-      <c r="E28" s="112">
+      <c r="E29" s="112">
         <v>55.053609132043469</v>
       </c>
-      <c r="F28" s="112">
+      <c r="F29" s="112">
         <v>55.053609132043469</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B29" s="101" t="s">
+    <row r="30" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B30" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="C29" s="112">
+      <c r="C30" s="112">
         <v>44.32</v>
       </c>
-      <c r="D29" s="111">
+      <c r="D30" s="111">
         <f t="shared" si="0"/>
         <v>48.326666666666668</v>
       </c>
-      <c r="E29" s="112">
+      <c r="E30" s="112">
         <v>56.34</v>
       </c>
-      <c r="F29" s="112">
+      <c r="F30" s="112">
         <v>56.34</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" t="s">
         <v>142</v>
       </c>
-      <c r="J29" s="101"/>
-      <c r="K29" s="112"/>
-      <c r="L29" s="111"/>
-      <c r="M29" s="112"/>
-      <c r="N29" s="112"/>
-    </row>
-    <row r="30" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B30" s="101" t="s">
+      <c r="J30" s="101"/>
+      <c r="K30" s="112"/>
+      <c r="L30" s="111"/>
+      <c r="M30" s="112"/>
+      <c r="N30" s="112"/>
+    </row>
+    <row r="31" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B31" s="101" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="112">
+      <c r="C31" s="112">
         <v>28.682639999999999</v>
       </c>
-      <c r="D30" s="121">
+      <c r="D31" s="111">
         <f t="shared" si="0"/>
         <v>28.682639999999999</v>
       </c>
-      <c r="E30" s="112">
+      <c r="E31" s="112">
         <v>28.682639999999999</v>
       </c>
-      <c r="F30" s="112">
+      <c r="F31" s="112">
         <v>28.682639999999999</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G31" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="2:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B31" s="109" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="110">
+    <row r="32" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B32" s="101" t="s">
+        <v>151</v>
+      </c>
+      <c r="C32" s="130">
+        <v>2.3699999999999999E-2</v>
+      </c>
+      <c r="D32" s="131">
+        <f t="shared" si="0"/>
+        <v>8.083333333333334E-2</v>
+      </c>
+      <c r="E32" s="130">
+        <v>0.1951</v>
+      </c>
+      <c r="F32" s="130">
+        <v>0.1951</v>
+      </c>
+      <c r="G32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B33" s="109" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="110">
         <v>1</v>
       </c>
-      <c r="D31" s="121">
+      <c r="D33" s="121">
         <f t="shared" si="0"/>
         <v>32.333333333333329</v>
       </c>
-      <c r="E31" s="110">
+      <c r="E33" s="110">
         <v>95</v>
       </c>
-      <c r="F31" s="110">
+      <c r="F33" s="110">
         <v>95</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G33" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="105" t="s">
+    <row r="34" spans="2:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="108">
+      <c r="C34" s="108">
         <v>170</v>
       </c>
-      <c r="D32" s="122">
+      <c r="D34" s="122">
         <f t="shared" si="0"/>
         <v>261.66666666666669</v>
       </c>
-      <c r="E32" s="108">
+      <c r="E34" s="108">
         <v>445</v>
       </c>
-      <c r="F32" s="108">
+      <c r="F34" s="108">
         <v>445</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G34" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3003,20 +3073,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="18" width="10.7109375" customWidth="1"/>
-    <col min="24" max="25" width="14.42578125" customWidth="1"/>
+    <col min="24" max="29" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -3092,11 +3162,23 @@
       <c r="Y1" s="42">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="42">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="42">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="42">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="42">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -3143,8 +3225,20 @@
       <c r="Y2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -3220,12 +3314,24 @@
       <c r="Y3" s="43">
         <v>0</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="43">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="43">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="43">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="43">
+        <v>0</v>
+      </c>
+      <c r="AD3">
         <f>SUM(B3:X3)*10^-6</f>
         <v>1.0341</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -3301,12 +3407,24 @@
       <c r="Y4" s="43">
         <v>0</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="43">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="43">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="43">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="43">
+        <v>0</v>
+      </c>
+      <c r="AD4">
         <f>SUM(B4:X4)*10^-6</f>
         <v>1.1751</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -3382,12 +3500,24 @@
       <c r="Y5" s="43">
         <v>0</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="43">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="43">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="43">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="43">
+        <v>0</v>
+      </c>
+      <c r="AD5">
         <f>SUM(B5:X5)*10^-6</f>
         <v>1.2790999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -3463,12 +3593,24 @@
       <c r="Y6" s="43">
         <v>0</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="43">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="43">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="43">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="43">
+        <v>0</v>
+      </c>
+      <c r="AD6">
         <f>SUM(B6:X6)*10^-6</f>
         <v>1.3346</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -3544,27 +3686,39 @@
       <c r="Y7" s="43">
         <v>0</v>
       </c>
-      <c r="Z7">
+      <c r="Z7" s="43">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="43">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="43">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="43">
+        <v>0</v>
+      </c>
+      <c r="AD7">
         <f>SUM(B7:X7)*10^-6</f>
         <v>1.351129</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
       <c r="B11" s="13"/>
       <c r="C11" s="43"/>
@@ -3580,7 +3734,7 @@
       <c r="M11" s="43"/>
       <c r="N11" s="43"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="13"/>
       <c r="C12" s="43"/>
@@ -3592,7 +3746,7 @@
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="42"/>
       <c r="B13" s="13"/>
       <c r="C13" s="43"/>
@@ -3604,7 +3758,7 @@
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="42"/>
       <c r="B14" s="13"/>
       <c r="C14" s="43"/>
@@ -3619,7 +3773,7 @@
       <c r="L14" s="43"/>
       <c r="M14" s="43"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="42"/>
       <c r="B15" s="13"/>
       <c r="C15" s="43"/>
@@ -3631,7 +3785,7 @@
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="42"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -4180,7 +4334,7 @@
       <c r="R12" s="91"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="126" t="s">
+      <c r="A13" s="128" t="s">
         <v>87</v>
       </c>
       <c r="B13" s="50" t="s">
@@ -4241,7 +4395,7 @@
       <c r="R13" s="91"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="126"/>
+      <c r="A14" s="128"/>
       <c r="B14" s="50" t="s">
         <v>44</v>
       </c>
@@ -4299,7 +4453,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="126"/>
+      <c r="A15" s="128"/>
       <c r="B15" s="50" t="s">
         <v>45</v>
       </c>
@@ -4357,7 +4511,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="126"/>
+      <c r="A16" s="128"/>
       <c r="B16" s="50" t="s">
         <v>46</v>
       </c>
@@ -4415,7 +4569,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="126"/>
+      <c r="A17" s="128"/>
       <c r="B17" s="50" t="s">
         <v>47</v>
       </c>
@@ -4473,7 +4627,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="127"/>
+      <c r="A18" s="129"/>
       <c r="B18" s="51" t="s">
         <v>48</v>
       </c>
@@ -5760,10 +5914,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K10"/>
+  <dimension ref="B1:K12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5772,6 +5926,7 @@
     <col min="2" max="2" width="6" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="35.5703125" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
@@ -6052,6 +6207,46 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="123">
+        <v>27</v>
+      </c>
+      <c r="C11" s="114" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" s="115">
+        <v>13.42</v>
+      </c>
+      <c r="E11" s="115">
+        <v>13.42</v>
+      </c>
+      <c r="F11" s="115">
+        <v>13.42</v>
+      </c>
+      <c r="G11" s="124" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="123">
+        <v>28</v>
+      </c>
+      <c r="C12" s="114" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="115">
+        <v>10.43</v>
+      </c>
+      <c r="E12" s="115">
+        <v>10.43</v>
+      </c>
+      <c r="F12" s="115">
+        <v>10.43</v>
+      </c>
+      <c r="G12" s="124" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added biomethane options from solid biomass for industrial processes. Changed the model starting year from 2015 to 2020. Added further climate targets (climate neutrality in 2045).
</commit_message>
<xml_diff>
--- a/src/Biomass_Data.xlsx
+++ b/src/Biomass_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="6480" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="6480"/>
   </bookViews>
   <sheets>
     <sheet name="Potentials" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,40 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="AD1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Quelle 2019: https://www.fnr.de/fileadmin/Projekte/2020/Mediathek/broschuere_basisdaten_bioenergie_2020_web.pdf</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autor</author>
@@ -731,7 +765,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -860,6 +894,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1064,7 +1111,7 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1340,6 +1387,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1353,12 +1407,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1767,8 +1815,8 @@
   </sheetPr>
   <dimension ref="B2:H35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,13 +1831,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
       <c r="G2" s="39"/>
     </row>
     <row r="3" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1943,7 +1991,7 @@
         <v>2.4</v>
       </c>
       <c r="D10" s="96">
-        <v>2.2999999999999998</v>
+        <v>2.34</v>
       </c>
       <c r="E10" s="96">
         <f>2.2*0.98</f>
@@ -1965,13 +2013,12 @@
       <c r="C11" s="97">
         <v>2.4</v>
       </c>
-      <c r="D11" s="97">
-        <f>0.75*C11</f>
-        <v>1.7999999999999998</v>
+      <c r="D11" s="96">
+        <v>2.34</v>
       </c>
       <c r="E11" s="97">
-        <f>0.5*C11*0.98</f>
-        <v>1.1759999999999999</v>
+        <f>0.67*C11*0.98</f>
+        <v>1.5758400000000001</v>
       </c>
       <c r="F11" s="97">
         <v>0</v>
@@ -1979,13 +2026,13 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="125" t="s">
+      <c r="B12" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="126"/>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="129"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:8" ht="21" x14ac:dyDescent="0.25">
@@ -2133,7 +2180,7 @@
         <v>2.4</v>
       </c>
       <c r="D20" s="96">
-        <v>2.2999999999999998</v>
+        <v>2.34</v>
       </c>
       <c r="E20" s="96">
         <f>2.2*0.96</f>
@@ -2155,25 +2202,24 @@
         <v>2.4</v>
       </c>
       <c r="D21" s="97">
-        <f>0.75*C21</f>
-        <v>1.7999999999999998</v>
+        <v>2.34</v>
       </c>
       <c r="E21" s="97">
-        <f>0.5*C21*0.96</f>
-        <v>1.1519999999999999</v>
+        <f>0.67*C21*0.96</f>
+        <v>1.5436799999999999</v>
       </c>
       <c r="F21" s="97">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="126" t="s">
+      <c r="B22" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="126"/>
-      <c r="D22" s="126"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="126"/>
+      <c r="C22" s="129"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="129"/>
+      <c r="F22" s="129"/>
       <c r="G22" s="11"/>
       <c r="H22" s="1"/>
     </row>
@@ -2260,7 +2306,10 @@
         <f>CulStart!AD7/Potentials!C10</f>
         <v>0.5629704166666667</v>
       </c>
-      <c r="D27" s="95"/>
+      <c r="D27" s="95">
+        <f>CulStart!AD8/Potentials!D10</f>
+        <v>0.61928589743589746</v>
+      </c>
       <c r="E27" s="94">
         <f>98*E25/100</f>
         <v>0.76439999999999997</v>
@@ -2278,7 +2327,10 @@
         <f>CulStart!AD7/Potentials!C11</f>
         <v>0.5629704166666667</v>
       </c>
-      <c r="D28" s="95"/>
+      <c r="D28" s="95">
+        <f>CulStart!AD8/Potentials!D11</f>
+        <v>0.61928589743589746</v>
+      </c>
       <c r="E28" s="94">
         <f>98*E25/100</f>
         <v>0.76439999999999997</v>
@@ -2289,13 +2341,13 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="127" t="s">
+      <c r="B29" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="127"/>
-      <c r="D29" s="127"/>
-      <c r="E29" s="127"/>
-      <c r="F29" s="127"/>
+      <c r="C29" s="130"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="130"/>
+      <c r="F29" s="130"/>
     </row>
     <row r="30" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
@@ -2378,7 +2430,10 @@
         <f>CulStart!AD7/Potentials!C20</f>
         <v>0.5629704166666667</v>
       </c>
-      <c r="D34" s="95"/>
+      <c r="D34" s="95">
+        <f>CulStart!AD8/Potentials!D20</f>
+        <v>0.61928589743589746</v>
+      </c>
       <c r="E34" s="94">
         <f>96*E32/100</f>
         <v>0.63359999999999994</v>
@@ -2396,7 +2451,10 @@
         <f>CulStart!AD7/Potentials!C21</f>
         <v>0.5629704166666667</v>
       </c>
-      <c r="D35" s="95"/>
+      <c r="D35" s="95">
+        <f>CulStart!AD8/Potentials!D21</f>
+        <v>0.61928589743589746</v>
+      </c>
       <c r="E35" s="94">
         <f>96*E32/100</f>
         <v>0.63359999999999994</v>
@@ -2423,8 +2481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2686,16 +2744,16 @@
       <c r="B14" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="C14" s="130">
+      <c r="C14" s="125">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D14" s="130">
+      <c r="D14" s="125">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E14" s="130">
+      <c r="E14" s="125">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F14" s="130">
+      <c r="F14" s="125">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G14" t="s">
@@ -3006,17 +3064,17 @@
       <c r="B32" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="C32" s="130">
+      <c r="C32" s="125">
         <v>2.3699999999999999E-2</v>
       </c>
-      <c r="D32" s="131">
+      <c r="D32" s="126">
         <f t="shared" si="0"/>
         <v>8.083333333333334E-2</v>
       </c>
-      <c r="E32" s="130">
+      <c r="E32" s="125">
         <v>0.1951</v>
       </c>
-      <c r="F32" s="130">
+      <c r="F32" s="125">
         <v>0.1951</v>
       </c>
       <c r="G32" t="s">
@@ -3072,11 +3130,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3327,7 +3385,7 @@
         <v>0</v>
       </c>
       <c r="AD3">
-        <f>SUM(B3:X3)*10^-6</f>
+        <f t="shared" ref="AD3:AD8" si="0">SUM(B3:X3)*10^-6</f>
         <v>1.0341</v>
       </c>
     </row>
@@ -3420,7 +3478,7 @@
         <v>0</v>
       </c>
       <c r="AD4">
-        <f>SUM(B4:X4)*10^-6</f>
+        <f t="shared" si="0"/>
         <v>1.1751</v>
       </c>
     </row>
@@ -3513,7 +3571,7 @@
         <v>0</v>
       </c>
       <c r="AD5">
-        <f>SUM(B5:X5)*10^-6</f>
+        <f t="shared" si="0"/>
         <v>1.2790999999999999</v>
       </c>
     </row>
@@ -3606,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="AD6">
-        <f>SUM(B6:X6)*10^-6</f>
+        <f t="shared" si="0"/>
         <v>1.3346</v>
       </c>
     </row>
@@ -3699,14 +3757,102 @@
         <v>0</v>
       </c>
       <c r="AD7">
-        <f>SUM(B7:X7)*10^-6</f>
+        <f t="shared" si="0"/>
         <v>1.351129</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="A8">
+        <v>2019</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0</v>
+      </c>
+      <c r="K8" s="43">
+        <v>970000</v>
+      </c>
+      <c r="L8" s="44">
+        <v>15600</v>
+      </c>
+      <c r="M8" s="44">
+        <v>6630</v>
+      </c>
+      <c r="N8" s="127">
+        <v>0</v>
+      </c>
+      <c r="O8" s="127">
+        <v>0</v>
+      </c>
+      <c r="P8" s="44">
+        <v>4500</v>
+      </c>
+      <c r="Q8" s="127">
+        <v>0</v>
+      </c>
+      <c r="R8" s="127">
+        <v>0</v>
+      </c>
+      <c r="S8" s="127">
+        <v>400</v>
+      </c>
+      <c r="T8" s="127">
+        <v>20150</v>
+      </c>
+      <c r="U8" s="44">
+        <v>0</v>
+      </c>
+      <c r="V8" s="127">
+        <v>157849</v>
+      </c>
+      <c r="W8" s="127">
+        <v>151000</v>
+      </c>
+      <c r="X8" s="127">
+        <v>123000</v>
+      </c>
+      <c r="Y8" s="43">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="43">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="43">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="43">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="43">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="0"/>
+        <v>1.4491289999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
@@ -3817,6 +3963,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4334,7 +4481,7 @@
       <c r="R12" s="91"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="128" t="s">
+      <c r="A13" s="131" t="s">
         <v>87</v>
       </c>
       <c r="B13" s="50" t="s">
@@ -4395,7 +4542,7 @@
       <c r="R13" s="91"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="128"/>
+      <c r="A14" s="131"/>
       <c r="B14" s="50" t="s">
         <v>44</v>
       </c>
@@ -4453,7 +4600,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="128"/>
+      <c r="A15" s="131"/>
       <c r="B15" s="50" t="s">
         <v>45</v>
       </c>
@@ -4511,7 +4658,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="128"/>
+      <c r="A16" s="131"/>
       <c r="B16" s="50" t="s">
         <v>46</v>
       </c>
@@ -4569,7 +4716,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="128"/>
+      <c r="A17" s="131"/>
       <c r="B17" s="50" t="s">
         <v>47</v>
       </c>
@@ -4627,7 +4774,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="129"/>
+      <c r="A18" s="132"/>
       <c r="B18" s="51" t="s">
         <v>48</v>
       </c>
@@ -5916,7 +6063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:G1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>